<commit_message>
updates to calendar, and posting initial schedule
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar-original(1-28-22).xlsx
+++ b/CS320-Spring2022Calendar-original(1-28-22).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D54B2FF-13A3-426C-AC6F-6201AC7DFF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C469711-1535-492C-8A1E-06CDA04E2E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="924" windowWidth="20844" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="366" yWindow="366" windowWidth="20844" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Monday</t>
   </si>
@@ -375,11 +375,6 @@
   </si>
   <si>
     <t>Feb / Mar</t>
-  </si>
-  <si>
-    <t>Library Example Project
-Analysis and
-Review (part 1)</t>
   </si>
   <si>
     <t>Mar / Apr</t>
@@ -506,15 +501,9 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Team Session
-(in class)
+      <t xml:space="preserve">Library Example Project
+Analysis and
+Review (part 1)
 </t>
     </r>
     <r>
@@ -526,9 +515,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-Exam (take home)
-due (in-class)</t>
+      <t>Take Home Exam
+(handed out</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
   <si>
@@ -547,9 +546,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-Exam (take home)
-(handed out)</t>
+      <t>Take Home Exam
+(due: in-class)</t>
     </r>
   </si>
 </sst>
@@ -1614,9 +1612,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1644,41 +1639,11 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1686,6 +1651,60 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1698,29 +1717,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2065,8 +2063,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2084,17 +2082,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="131"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2124,10 +2122,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="135">
+      <c r="A3" s="138">
         <v>15</v>
       </c>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="129" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="43">
@@ -2159,8 +2157,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="134"/>
-      <c r="B4" s="151"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="132"/>
       <c r="C4" s="41" t="s">
         <v>8</v>
       </c>
@@ -2186,11 +2184,11 @@
       <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="134">
+      <c r="A5" s="139">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="130" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="8">
@@ -2222,8 +2220,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="136"/>
-      <c r="B6" s="142"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="83"/>
       <c r="D6" s="75" t="s">
         <v>58</v>
@@ -2241,11 +2239,11 @@
       <c r="I6" s="85"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="137">
+      <c r="A7" s="143">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="150" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="63">
@@ -2278,8 +2276,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="140"/>
-      <c r="B8" s="144"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="151"/>
       <c r="C8" s="40" t="s">
         <v>43</v>
       </c>
@@ -2299,11 +2297,11 @@
       <c r="I8" s="79"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="140">
+      <c r="A9" s="136">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="144"/>
+      <c r="B9" s="151"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2334,8 +2332,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="140"/>
-      <c r="B10" s="144"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="151"/>
       <c r="C10" s="40" t="s">
         <v>55</v>
       </c>
@@ -2353,11 +2351,11 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="140">
+      <c r="A11" s="136">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="144"/>
+      <c r="B11" s="151"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2388,8 +2386,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="140"/>
-      <c r="B12" s="144"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="151"/>
       <c r="C12" s="38"/>
       <c r="D12" s="33" t="s">
         <v>32</v>
@@ -2405,11 +2403,11 @@
       <c r="I12" s="104"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="145">
+      <c r="A13" s="152">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="133" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="18">
@@ -2441,8 +2439,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="146"/>
-      <c r="B14" s="153"/>
+      <c r="A14" s="153"/>
+      <c r="B14" s="134"/>
       <c r="C14" s="38"/>
       <c r="D14" s="99" t="s">
         <v>26</v>
@@ -2453,16 +2451,16 @@
       </c>
       <c r="G14" s="94"/>
       <c r="H14" s="61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I14" s="95"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="135">
+      <c r="A15" s="138">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="90">
@@ -2495,15 +2493,15 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="136"/>
-      <c r="B16" s="142"/>
+      <c r="A16" s="142"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="93" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="127" t="s">
+      <c r="E16" s="126" t="s">
         <v>60</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -2599,8 +2597,8 @@
       <c r="B23" s="27"/>
       <c r="C23" s="52"/>
       <c r="D23" s="30"/>
-      <c r="E23" s="126" t="s">
-        <v>68</v>
+      <c r="E23" s="125" t="s">
+        <v>67</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2652,19 +2650,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="129" t="str">
+      <c r="A28" s="145" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
 (as of 12-27-2021, subject to change)</v>
       </c>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="131"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="147"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2702,11 +2700,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="132">
+      <c r="A30" s="148">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="150" t="s">
+      <c r="B30" s="129" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="107">
@@ -2739,8 +2737,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="133"/>
-      <c r="B31" s="141"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="107" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
@@ -2774,11 +2772,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="133">
+      <c r="A32" s="149">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="141"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="68">
         <f>I15 + 1</f>
         <v>13</v>
@@ -2809,10 +2807,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="134"/>
-      <c r="B33" s="141"/>
+      <c r="A33" s="139"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>37</v>
@@ -2828,11 +2826,11 @@
       <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="134">
+      <c r="A34" s="139">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="141"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2863,29 +2861,29 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="120.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="134"/>
-      <c r="B35" s="141"/>
+      <c r="A35" s="139"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="80"/>
       <c r="D35" s="24" t="s">
         <v>15</v>
       </c>
       <c r="E35" s="96"/>
       <c r="F35" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="80"/>
+      <c r="H35" s="127" t="s">
         <v>70</v>
       </c>
-      <c r="G35" s="80"/>
-      <c r="H35" s="128" t="s">
-        <v>71</v>
-      </c>
       <c r="I35" s="116"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="134">
+      <c r="A36" s="139">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="154" t="s">
-        <v>65</v>
+      <c r="B36" s="135" t="s">
+        <v>64</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2916,8 +2914,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="136"/>
-      <c r="B37" s="142"/>
+      <c r="A37" s="142"/>
+      <c r="B37" s="131"/>
       <c r="C37" s="113"/>
       <c r="D37" s="114" t="s">
         <v>38</v>
@@ -2937,11 +2935,11 @@
       <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="137">
+      <c r="A38" s="143">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="149" t="s">
+      <c r="B38" s="128" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="111">
@@ -2974,8 +2972,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="140"/>
-      <c r="B39" s="149"/>
+      <c r="A39" s="136"/>
+      <c r="B39" s="128"/>
       <c r="C39" s="118"/>
       <c r="D39" s="24" t="s">
         <v>29</v>
@@ -2984,20 +2982,20 @@
         <v>45</v>
       </c>
       <c r="F39" s="60" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G39" s="60"/>
-      <c r="H39" s="60" t="s">
-        <v>73</v>
+      <c r="H39" s="154" t="s">
+        <v>72</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="139">
+      <c r="A40" s="144">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="149"/>
+      <c r="B40" s="128"/>
       <c r="C40" s="117">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3027,12 +3025,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="140"/>
-      <c r="B41" s="149"/>
+    <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="136"/>
+      <c r="B41" s="128"/>
       <c r="C41" s="38"/>
-      <c r="D41" s="119" t="s">
-        <v>72</v>
+      <c r="D41" s="36" t="s">
+        <v>7</v>
       </c>
       <c r="E41" s="74"/>
       <c r="F41" s="23" t="s">
@@ -3047,11 +3045,11 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="140">
+      <c r="A42" s="136">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="149"/>
+      <c r="B42" s="128"/>
       <c r="C42" s="42">
         <f>I40 + 1</f>
         <v>17</v>
@@ -3082,8 +3080,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="140"/>
-      <c r="B43" s="149"/>
+      <c r="A43" s="136"/>
+      <c r="B43" s="128"/>
       <c r="C43" s="41" t="s">
         <v>6</v>
       </c>
@@ -3101,11 +3099,11 @@
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="140">
+      <c r="A44" s="136">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="149"/>
+      <c r="B44" s="128"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3136,8 +3134,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="138"/>
-      <c r="B45" s="149"/>
+      <c r="A45" s="137"/>
+      <c r="B45" s="128"/>
       <c r="C45" s="108"/>
       <c r="D45" s="69" t="s">
         <v>31</v>
@@ -3153,11 +3151,11 @@
       <c r="I45" s="66"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="135">
+      <c r="A46" s="138">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="150" t="s">
+      <c r="B46" s="129" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3189,8 +3187,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="134"/>
-      <c r="B47" s="141"/>
+      <c r="A47" s="139"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3201,17 +3199,17 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I47" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="147" t="s">
+      <c r="A48" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="141"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3232,50 +3230,35 @@
         <f t="shared" si="14"/>
         <v>12</v>
       </c>
-      <c r="H48" s="122">
+      <c r="H48" s="121">
         <f t="shared" si="14"/>
         <v>13</v>
       </c>
-      <c r="I48" s="123">
+      <c r="I48" s="122">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="148"/>
-      <c r="B49" s="142"/>
-      <c r="C49" s="120" t="s">
+      <c r="A49" s="141"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="119" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="121"/>
+      <c r="E49" s="120"/>
       <c r="F49" s="25" t="s">
         <v>39</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="124"/>
-      <c r="I49" s="125"/>
+      <c r="H49" s="123"/>
+      <c r="I49" s="124"/>
     </row>
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3289,6 +3272,21 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated calendar and assignment dates
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar-original(1-28-22).xlsx
+++ b/CS320-Spring2022Calendar-original(1-28-22).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C469711-1535-492C-8A1E-06CDA04E2E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EC85D7-DFCC-4D04-9C83-0997607A1D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="366" yWindow="366" windowWidth="20844" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1098" yWindow="924" windowWidth="20844" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -188,18 +188,6 @@
   </si>
   <si>
     <t>A04: Individual MS3 Final Project Demo</t>
-  </si>
-  <si>
-    <t>FINAL EXAM PERIOD
-101: 8:00-10:00 102: 10:15-12:15
-A08: Team Presentation and Demonstration
-(in class)</t>
-  </si>
-  <si>
-    <t>FINAL EXAM PERIOD
-103: 3:00-5:00
-A08: Team Presentation and Demonstration
-(in class)</t>
   </si>
   <si>
     <t>Lab 1: HTML &amp; CSS  due
@@ -549,6 +537,19 @@
       <t>Take Home Exam
 (due: in-class)</t>
     </r>
+  </si>
+  <si>
+    <t>FINAL EXAM PERIOD
+101: 8:00-10:00
+103: 3:00-5:00
+A08: Team Presentation and Demonstration
+(in class)</t>
+  </si>
+  <si>
+    <t>FINAL EXAM PERIOD
+102: 10:15-12:15
+A08: Team Presentation and Demonstration
+(in class)</t>
   </si>
 </sst>
 </file>
@@ -1639,18 +1640,75 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1662,63 +1720,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2063,8 +2064,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2082,17 +2083,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="145" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="147"/>
+      <c r="A1" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="131"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2122,10 +2123,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="138">
+      <c r="A3" s="135">
         <v>15</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="150" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="43">
@@ -2157,8 +2158,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="139"/>
-      <c r="B4" s="132"/>
+      <c r="A4" s="134"/>
+      <c r="B4" s="151"/>
       <c r="C4" s="41" t="s">
         <v>8</v>
       </c>
@@ -2184,12 +2185,12 @@
       <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="139">
+      <c r="A5" s="134">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="130" t="s">
-        <v>62</v>
+      <c r="B5" s="139" t="s">
+        <v>60</v>
       </c>
       <c r="C5" s="8">
         <f>I3 + 1</f>
@@ -2220,30 +2221,30 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="142"/>
-      <c r="B6" s="131"/>
+      <c r="A6" s="136"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="83"/>
       <c r="D6" s="75" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="105"/>
       <c r="F6" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" s="73" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I6" s="85"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="143">
+      <c r="A7" s="137">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="63">
@@ -2276,32 +2277,32 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="136"/>
-      <c r="B8" s="151"/>
+      <c r="A8" s="138"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="60"/>
       <c r="F8" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H8" s="60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I8" s="79"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="136">
+      <c r="A9" s="138">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="151"/>
+      <c r="B9" s="142"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2332,10 +2333,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="136"/>
-      <c r="B10" s="151"/>
+      <c r="A10" s="138"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>25</v>
@@ -2351,11 +2352,11 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="136">
+      <c r="A11" s="138">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="151"/>
+      <c r="B11" s="142"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2386,8 +2387,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="136"/>
-      <c r="B12" s="151"/>
+      <c r="A12" s="138"/>
+      <c r="B12" s="142"/>
       <c r="C12" s="38"/>
       <c r="D12" s="33" t="s">
         <v>32</v>
@@ -2403,12 +2404,12 @@
       <c r="I12" s="104"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="152">
+      <c r="A13" s="143">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="133" t="s">
-        <v>63</v>
+      <c r="B13" s="152" t="s">
+        <v>61</v>
       </c>
       <c r="C13" s="18">
         <f>I11 + 1</f>
@@ -2439,28 +2440,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="153"/>
-      <c r="B14" s="134"/>
+      <c r="A14" s="144"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="38"/>
       <c r="D14" s="99" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="98"/>
       <c r="F14" s="77" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="94"/>
       <c r="H14" s="61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14" s="95"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="138">
+      <c r="A15" s="135">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="139" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="90">
@@ -2493,22 +2494,22 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="142"/>
-      <c r="B16" s="131"/>
+      <c r="A16" s="136"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="93" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="126" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H16" s="49" t="str">
         <f>G16</f>
@@ -2598,7 +2599,7 @@
       <c r="C23" s="52"/>
       <c r="D23" s="30"/>
       <c r="E23" s="125" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2650,19 +2651,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="145" t="str">
+      <c r="A28" s="129" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
 (as of 12-27-2021, subject to change)</v>
       </c>
-      <c r="B28" s="146"/>
-      <c r="C28" s="146"/>
-      <c r="D28" s="146"/>
-      <c r="E28" s="146"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="146"/>
-      <c r="H28" s="146"/>
-      <c r="I28" s="147"/>
+      <c r="B28" s="130"/>
+      <c r="C28" s="130"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="131"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2700,11 +2701,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="148">
+      <c r="A30" s="132">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="129" t="s">
+      <c r="B30" s="150" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="107">
@@ -2737,8 +2738,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="149"/>
-      <c r="B31" s="130"/>
+      <c r="A31" s="133"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="107" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
@@ -2772,11 +2773,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="149">
+      <c r="A32" s="133">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="130"/>
+      <c r="B32" s="139"/>
       <c r="C32" s="68">
         <f>I15 + 1</f>
         <v>13</v>
@@ -2807,10 +2808,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="139"/>
-      <c r="B33" s="130"/>
+      <c r="A33" s="134"/>
+      <c r="B33" s="139"/>
       <c r="C33" s="40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D33" s="33" t="s">
         <v>37</v>
@@ -2826,11 +2827,11 @@
       <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="139">
+      <c r="A34" s="134">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="130"/>
+      <c r="B34" s="139"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2861,29 +2862,29 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="120.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="139"/>
-      <c r="B35" s="130"/>
+      <c r="A35" s="134"/>
+      <c r="B35" s="139"/>
       <c r="C35" s="80"/>
       <c r="D35" s="24" t="s">
         <v>15</v>
       </c>
       <c r="E35" s="96"/>
       <c r="F35" s="73" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G35" s="80"/>
       <c r="H35" s="127" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I35" s="116"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="139">
+      <c r="A36" s="134">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="135" t="s">
-        <v>64</v>
+      <c r="B36" s="154" t="s">
+        <v>62</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2914,32 +2915,32 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="142"/>
-      <c r="B37" s="131"/>
+      <c r="A37" s="136"/>
+      <c r="B37" s="140"/>
       <c r="C37" s="113"/>
       <c r="D37" s="114" t="s">
         <v>38</v>
       </c>
       <c r="E37" s="115" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="78" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H37" s="60" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="143">
+      <c r="A38" s="137">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="128" t="s">
+      <c r="B38" s="149" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="111">
@@ -2972,30 +2973,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="136"/>
-      <c r="B39" s="128"/>
+      <c r="A39" s="138"/>
+      <c r="B39" s="149"/>
       <c r="C39" s="118"/>
       <c r="D39" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E39" s="81" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F39" s="60" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G39" s="60"/>
-      <c r="H39" s="154" t="s">
-        <v>72</v>
+      <c r="H39" s="128" t="s">
+        <v>70</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="144">
+      <c r="A40" s="148">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="128"/>
+      <c r="B40" s="149"/>
       <c r="C40" s="117">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3026,8 +3027,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="136"/>
-      <c r="B41" s="128"/>
+      <c r="A41" s="138"/>
+      <c r="B41" s="149"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
@@ -3045,11 +3046,11 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="136">
+      <c r="A42" s="138">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="128"/>
+      <c r="B42" s="149"/>
       <c r="C42" s="42">
         <f>I40 + 1</f>
         <v>17</v>
@@ -3080,8 +3081,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="136"/>
-      <c r="B43" s="128"/>
+      <c r="A43" s="138"/>
+      <c r="B43" s="149"/>
       <c r="C43" s="41" t="s">
         <v>6</v>
       </c>
@@ -3099,11 +3100,11 @@
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="136">
+      <c r="A44" s="138">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="128"/>
+      <c r="B44" s="149"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3134,8 +3135,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="137"/>
-      <c r="B45" s="128"/>
+      <c r="A45" s="145"/>
+      <c r="B45" s="149"/>
       <c r="C45" s="108"/>
       <c r="D45" s="69" t="s">
         <v>31</v>
@@ -3151,11 +3152,11 @@
       <c r="I45" s="66"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="138">
+      <c r="A46" s="135">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="129" t="s">
+      <c r="B46" s="150" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3187,8 +3188,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="139"/>
-      <c r="B47" s="130"/>
+      <c r="A47" s="134"/>
+      <c r="B47" s="139"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3199,17 +3200,17 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="140" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="130"/>
+      <c r="A48" s="146" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="139"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3240,17 +3241,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="141"/>
-      <c r="B49" s="131"/>
+      <c r="A49" s="147"/>
+      <c r="B49" s="140"/>
       <c r="C49" s="119" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="E49" s="120"/>
       <c r="F49" s="25" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="123"/>
@@ -3259,6 +3260,21 @@
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3272,21 +3288,6 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed Ind and Team MS dates
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar-original(1-28-22).xlsx
+++ b/CS320-Spring2022Calendar-original(1-28-22).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EC85D7-DFCC-4D04-9C83-0997607A1D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3F93A1-CF5F-4F5E-9986-B8E78984449F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1098" yWindow="924" windowWidth="20844" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9192" yWindow="546" windowWidth="13758" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>Monday</t>
   </si>
@@ -205,9 +205,6 @@
 (Google Doc)</t>
   </si>
   <si>
-    <t>Lab 6: ORM due  7:00 am (Marmoset)</t>
-  </si>
-  <si>
     <t>A11: Team Project Midterm
 Peer Evals due
 7:00 am
@@ -227,9 +224,6 @@
 A11: Team Project
 Final Self/Peer Evaluations due
 both 7:00 am (Marmoset)</t>
-  </si>
-  <si>
-    <t>Work Ethic Lecture</t>
   </si>
   <si>
     <t>Final Presentation &amp; Demo</t>
@@ -353,10 +347,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2022 Schedule
-(as of 12-27-2021, subject to change)</t>
   </si>
   <si>
     <t>Jan / Feb</t>
@@ -550,6 +540,34 @@
 102: 10:15-12:15
 A08: Team Presentation and Demonstration
 (in class)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Work Ethic Lecture</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Lab 6: ORM due  7:00 am (Marmoset)</t>
+    </r>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2022 Schedule
+(as of 12-29-2021, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -663,12 +681,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -691,8 +703,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1061,19 +1079,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -1257,7 +1262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1328,36 +1333,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1373,43 +1378,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1418,18 +1390,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1451,19 +1420,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1475,7 +1441,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1487,10 +1453,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1499,18 +1462,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1520,10 +1477,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1538,10 +1495,10 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1550,46 +1507,40 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1598,80 +1549,38 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1679,6 +1588,60 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1688,38 +1651,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2065,7 +2067,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2083,17 +2085,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="129" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="131"/>
+      <c r="A1" s="122" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="124"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2123,24 +2125,24 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="135">
+      <c r="A3" s="115">
         <v>15</v>
       </c>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="141">
         <v>23</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="135">
         <f>C3 + 1</f>
         <v>24</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="135">
         <f t="shared" ref="E3:I3" si="0">D3 + 1</f>
         <v>25</v>
       </c>
-      <c r="F3" s="82">
+      <c r="F3" s="142">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
@@ -2158,39 +2160,39 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="134"/>
-      <c r="B4" s="151"/>
-      <c r="C4" s="41" t="s">
+      <c r="A4" s="116"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="42" t="str">
-        <f>C4</f>
+      <c r="D4" s="138" t="str">
+        <f xml:space="preserve"> C4</f>
         <v>SEMESTER
 BREAK</v>
       </c>
-      <c r="E4" s="84" t="str">
+      <c r="E4" s="144" t="str">
         <f>D4</f>
         <v>SEMESTER
 BREAK</v>
       </c>
-      <c r="F4" s="106" t="str">
+      <c r="F4" s="145" t="str">
         <f>E4</f>
         <v>SEMESTER
 BREAK</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="61" t="s">
+      <c r="G4" s="50"/>
+      <c r="H4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="65"/>
+      <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="134">
+      <c r="A5" s="116">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="139" t="s">
-        <v>60</v>
+      <c r="B5" s="107" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="8">
         <f>I3 + 1</f>
@@ -2200,70 +2202,70 @@
         <f>C5 + 1</f>
         <v>31</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="51">
         <v>1</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="52">
         <f t="shared" ref="E5:I13" si="1">E5 + 1</f>
         <v>2</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="52">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H5" s="64">
+      <c r="H5" s="52">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I5" s="72">
+      <c r="I5" s="59">
         <f>H5 + 1</f>
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="136"/>
-      <c r="B6" s="140"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="75" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="105"/>
+      <c r="A6" s="119"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="88"/>
       <c r="F6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="85"/>
+      <c r="H6" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="137">
+      <c r="A7" s="120">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="63">
+      <c r="C7" s="51">
         <f>I5 + 1</f>
         <v>6</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="52">
         <f>C7 + 1</f>
         <v>7</v>
       </c>
-      <c r="E7" s="87">
+      <c r="E7" s="71">
         <f>D7 + 1</f>
         <v>8</v>
       </c>
-      <c r="F7" s="88">
+      <c r="F7" s="72">
         <f>E7+1</f>
         <v>9</v>
       </c>
-      <c r="G7" s="89">
+      <c r="G7" s="73">
         <f>F7+1</f>
         <v>10</v>
       </c>
@@ -2271,38 +2273,38 @@
         <f>G7 + 1</f>
         <v>11</v>
       </c>
-      <c r="I7" s="86">
+      <c r="I7" s="70">
         <f>H7+1</f>
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="138"/>
-      <c r="B8" s="142"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="128"/>
       <c r="C8" s="40" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="60"/>
+        <v>53</v>
+      </c>
+      <c r="E8" s="48"/>
       <c r="F8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="79"/>
+      <c r="H8" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="138">
+      <c r="A9" s="113">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="142"/>
+      <c r="B9" s="128"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2333,16 +2335,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="138"/>
-      <c r="B10" s="142"/>
+      <c r="A10" s="113"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="48" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="48" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="12"/>
@@ -2352,11 +2354,11 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="138">
+      <c r="A11" s="113">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="142"/>
+      <c r="B11" s="128"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2387,46 +2389,46 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="138"/>
-      <c r="B12" s="142"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="128"/>
       <c r="C12" s="38"/>
-      <c r="D12" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="102"/>
-      <c r="F12" s="103" t="s">
+      <c r="D12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="102"/>
-      <c r="H12" s="76" t="s">
+      <c r="E12" s="63"/>
+      <c r="F12" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="104"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="87"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="143">
+      <c r="A13" s="129">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="152" t="s">
-        <v>61</v>
+      <c r="B13" s="110" t="s">
+        <v>58</v>
       </c>
       <c r="C13" s="18">
         <f>I11 + 1</f>
         <v>27</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="70">
         <f>C13 + 1</f>
         <v>28</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="84">
         <v>1</v>
       </c>
       <c r="F13" s="19">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="85">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2434,96 +2436,96 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I13" s="92">
+      <c r="I13" s="76">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="144"/>
-      <c r="B14" s="153"/>
+      <c r="A14" s="130"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="38"/>
-      <c r="D14" s="99" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="98"/>
-      <c r="F14" s="77" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="94"/>
-      <c r="H14" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="95"/>
+      <c r="D14" s="131" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="82"/>
+      <c r="F14" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="78"/>
+      <c r="H14" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="135">
+      <c r="A15" s="115">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="139" t="s">
+      <c r="B15" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="90">
+      <c r="C15" s="74">
         <f>I13 + 1</f>
         <v>6</v>
       </c>
-      <c r="D15" s="91">
+      <c r="D15" s="75">
         <f t="shared" ref="D15:I15" si="2">C15 + 1</f>
         <v>7</v>
       </c>
-      <c r="E15" s="96">
+      <c r="E15" s="80">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="F15" s="97">
+      <c r="F15" s="81">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G15" s="137">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="138">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="I15" s="45">
+      <c r="I15" s="139">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="136"/>
-      <c r="B16" s="140"/>
-      <c r="C16" s="93" t="s">
-        <v>58</v>
+      <c r="A16" s="119"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="77" t="s">
+        <v>56</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="126" t="s">
-        <v>58</v>
+      <c r="E16" s="102" t="s">
+        <v>56</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="49" t="str">
+      <c r="G16" s="146" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="147" t="str">
         <f>G16</f>
         <v>WINTER
 BREAK</v>
       </c>
-      <c r="I16" s="48" t="str">
+      <c r="I16" s="148" t="str">
         <f>H16</f>
         <v>WINTER
 BREAK</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="31" customFormat="1" ht="20.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="53"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="27"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -2534,10 +2536,10 @@
       <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" s="31" customFormat="1" ht="20.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="53"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="27"/>
       <c r="D18" s="30"/>
-      <c r="E18" s="58" t="s">
+      <c r="E18" s="46" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="30"/>
@@ -2546,10 +2548,10 @@
       <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" s="29" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="53"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="32"/>
       <c r="D19" s="26"/>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="149" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="26"/>
@@ -2558,10 +2560,10 @@
       <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" s="31" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="53"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="27"/>
       <c r="D20" s="30"/>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="43" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="30"/>
@@ -2570,10 +2572,10 @@
       <c r="I20" s="30"/>
     </row>
     <row r="21" spans="1:9" s="31" customFormat="1" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="53"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="27"/>
       <c r="D21" s="30"/>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="44" t="s">
         <v>23</v>
       </c>
       <c r="F21" s="30"/>
@@ -2582,10 +2584,10 @@
       <c r="I21" s="30"/>
     </row>
     <row r="22" spans="1:9" s="31" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="53"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="27"/>
       <c r="D22" s="30"/>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="45" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="30"/>
@@ -2594,12 +2596,12 @@
       <c r="I22" s="30"/>
     </row>
     <row r="23" spans="1:9" s="31" customFormat="1" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="53"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="27"/>
-      <c r="C23" s="52"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="30"/>
-      <c r="E23" s="125" t="s">
-        <v>65</v>
+      <c r="E23" s="101" t="s">
+        <v>62</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2607,7 +2609,7 @@
       <c r="I23" s="30"/>
     </row>
     <row r="24" spans="1:9" s="29" customFormat="1" ht="20.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="53"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="32"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -2618,7 +2620,7 @@
       <c r="I24" s="26"/>
     </row>
     <row r="25" spans="1:9" s="29" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="53"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="32"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -2629,7 +2631,7 @@
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" s="29" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="53"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="32"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
@@ -2640,7 +2642,7 @@
       <c r="I26" s="26"/>
     </row>
     <row r="27" spans="1:9" s="29" customFormat="1" ht="20.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="53"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="32"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
@@ -2651,19 +2653,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="129" t="str">
+      <c r="A28" s="122" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
-(as of 12-27-2021, subject to change)</v>
-      </c>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="131"/>
+(as of 12-29-2021, subject to change)</v>
+      </c>
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="123"/>
+      <c r="I28" s="124"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2701,84 +2703,84 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="132">
+      <c r="A30" s="125">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="150" t="s">
+      <c r="B30" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="107">
+      <c r="C30" s="89">
         <f t="shared" ref="C30:E30" si="4">C15</f>
         <v>6</v>
       </c>
-      <c r="D30" s="97">
+      <c r="D30" s="81">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="E30" s="96">
+      <c r="E30" s="80">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="F30" s="91">
+      <c r="F30" s="75">
         <f>F15</f>
         <v>9</v>
       </c>
-      <c r="G30" s="50">
+      <c r="G30" s="134">
         <f>G15</f>
         <v>10</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="135">
         <f>H15</f>
         <v>11</v>
       </c>
-      <c r="I30" s="46">
+      <c r="I30" s="136">
         <f>I15</f>
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="133"/>
-      <c r="B31" s="139"/>
-      <c r="C31" s="107" t="str">
+      <c r="A31" s="126"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="89" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D31" s="97" t="str">
+      <c r="D31" s="81" t="str">
         <f t="shared" ref="D31:H31" si="5">D16</f>
         <v>Lecture 16: Testing</v>
       </c>
-      <c r="E31" s="96" t="str">
+      <c r="E31" s="80" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F31" s="97" t="str">
+      <c r="F31" s="81" t="str">
         <f t="shared" si="5"/>
         <v>Lecture 17: Code Quality</v>
       </c>
-      <c r="G31" s="51" t="str">
+      <c r="G31" s="137" t="str">
         <f t="shared" si="5"/>
         <v>WINTER
 BREAK</v>
       </c>
-      <c r="H31" s="42" t="str">
+      <c r="H31" s="138" t="str">
         <f t="shared" si="5"/>
         <v>WINTER
 BREAK</v>
       </c>
-      <c r="I31" s="45" t="str">
+      <c r="I31" s="139" t="str">
         <f>I16</f>
         <v>WINTER
 BREAK</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="133">
+      <c r="A32" s="126">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="139"/>
-      <c r="C32" s="68">
+      <c r="B32" s="107"/>
+      <c r="C32" s="140">
         <f>I15 + 1</f>
         <v>13</v>
       </c>
@@ -2808,13 +2810,13 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="134"/>
-      <c r="B33" s="139"/>
+      <c r="A33" s="116"/>
+      <c r="B33" s="107"/>
       <c r="C33" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>37</v>
+        <v>61</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7" t="s">
@@ -2824,14 +2826,14 @@
       <c r="H33" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I33" s="59"/>
+      <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="134">
+      <c r="A34" s="116">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="139"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2862,29 +2864,29 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="120.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="134"/>
-      <c r="B35" s="139"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="96"/>
-      <c r="F35" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="80"/>
-      <c r="H35" s="127" t="s">
-        <v>68</v>
-      </c>
-      <c r="I35" s="116"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="80"/>
+      <c r="F35" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="66"/>
+      <c r="H35" s="103" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="96"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="134">
+      <c r="A36" s="116">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="154" t="s">
-        <v>62</v>
+      <c r="B36" s="112" t="s">
+        <v>59</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2906,102 +2908,100 @@
         <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="H36" s="88">
+      <c r="H36" s="72">
         <v>1</v>
       </c>
-      <c r="I36" s="112">
+      <c r="I36" s="94">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="136"/>
-      <c r="B37" s="140"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="114" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="115" t="s">
-        <v>44</v>
+      <c r="A37" s="119"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="67" t="s">
+        <v>42</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="H37" s="60" t="s">
-        <v>47</v>
+      <c r="G37" s="96"/>
+      <c r="H37" s="133" t="s">
+        <v>70</v>
       </c>
       <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="137">
+      <c r="A38" s="120">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="149" t="s">
+      <c r="B38" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="111">
+      <c r="C38" s="93">
         <f>I36 + 1</f>
         <v>3</v>
       </c>
-      <c r="D38" s="87">
+      <c r="D38" s="71">
         <f>C38+1</f>
         <v>4</v>
       </c>
-      <c r="E38" s="64">
+      <c r="E38" s="52">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="F38" s="88">
+      <c r="F38" s="72">
         <f>E38 + 1</f>
         <v>6</v>
       </c>
-      <c r="G38" s="71">
+      <c r="G38" s="58">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="H38" s="87">
+      <c r="H38" s="71">
         <f>G38 + 1</f>
         <v>8</v>
       </c>
-      <c r="I38" s="110">
+      <c r="I38" s="92">
         <f>H38 + 1</f>
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="138"/>
-      <c r="B39" s="149"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="81" t="s">
+      <c r="A39" s="113"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="60"/>
-      <c r="H39" s="128" t="s">
-        <v>70</v>
+      <c r="F39" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="132"/>
+      <c r="H39" s="104" t="s">
+        <v>67</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="148">
+      <c r="A40" s="121">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="149"/>
-      <c r="C40" s="117">
+      <c r="B40" s="105"/>
+      <c r="C40" s="97">
         <f>I38 + 1</f>
         <v>10</v>
       </c>
-      <c r="D40" s="71">
+      <c r="D40" s="58">
         <f>C40 + 1</f>
         <v>11</v>
       </c>
@@ -3013,49 +3013,49 @@
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="G40" s="36">
+      <c r="G40" s="58">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="H40" s="42">
+      <c r="H40" s="138">
         <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="I40" s="45">
+      <c r="I40" s="139">
         <f t="shared" si="9"/>
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="138"/>
-      <c r="B41" s="149"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="74"/>
+      <c r="E41" s="61"/>
       <c r="F41" s="23" t="s">
         <v>7</v>
       </c>
       <c r="G41" s="36"/>
-      <c r="H41" s="42" t="s">
+      <c r="H41" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="45" t="s">
+      <c r="I41" s="139" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="138">
+      <c r="A42" s="113">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="149"/>
-      <c r="C42" s="42">
+      <c r="B42" s="105"/>
+      <c r="C42" s="138">
         <f>I40 + 1</f>
         <v>17</v>
       </c>
-      <c r="D42" s="42">
+      <c r="D42" s="138">
         <f>C42 + 1</f>
         <v>18</v>
       </c>
@@ -3080,18 +3080,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="138"/>
-      <c r="B43" s="149"/>
-      <c r="C43" s="41" t="s">
+    <row r="43" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="113"/>
+      <c r="B43" s="105"/>
+      <c r="C43" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="51" t="s">
+      <c r="D43" s="137" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="12"/>
-      <c r="F43" s="23" t="s">
-        <v>7</v>
+      <c r="F43" s="56" t="s">
+        <v>31</v>
       </c>
       <c r="G43" s="23"/>
       <c r="H43" s="23" t="s">
@@ -3100,11 +3100,11 @@
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="138">
+      <c r="A44" s="113">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="149"/>
+      <c r="B44" s="105"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3135,28 +3135,26 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="145"/>
-      <c r="B45" s="149"/>
-      <c r="C45" s="108"/>
-      <c r="D45" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" s="67"/>
-      <c r="F45" s="70" t="s">
+      <c r="A45" s="114"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="67"/>
-      <c r="H45" s="70" t="s">
+      <c r="G45" s="55"/>
+      <c r="H45" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="66"/>
+      <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="135">
+      <c r="A46" s="115">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="150" t="s">
+      <c r="B46" s="106" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3166,11 +3164,11 @@
         <f>C46 + 1</f>
         <v>2</v>
       </c>
-      <c r="E46" s="109">
+      <c r="E46" s="91">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="F46" s="109">
+      <c r="F46" s="91">
         <f t="shared" ref="F46" si="12">E46 + 1</f>
         <v>4</v>
       </c>
@@ -3188,29 +3186,29 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="134"/>
-      <c r="B47" s="139"/>
+      <c r="A47" s="116"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="80"/>
+      <c r="E47" s="66"/>
       <c r="F47" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="146" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="139"/>
+      <c r="A48" s="117" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="107"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3219,7 +3217,7 @@
         <f t="shared" ref="D48:I48" si="14">C48 + 1</f>
         <v>9</v>
       </c>
-      <c r="E48" s="100">
+      <c r="E48" s="84">
         <f t="shared" si="14"/>
         <v>10</v>
       </c>
@@ -3231,50 +3229,35 @@
         <f t="shared" si="14"/>
         <v>12</v>
       </c>
-      <c r="H48" s="121">
+      <c r="H48" s="150">
         <f t="shared" si="14"/>
         <v>13</v>
       </c>
-      <c r="I48" s="122">
+      <c r="I48" s="151">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="147"/>
-      <c r="B49" s="140"/>
-      <c r="C49" s="119" t="s">
-        <v>46</v>
+      <c r="A49" s="118"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="99" t="s">
+        <v>45</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" s="120"/>
+        <v>68</v>
+      </c>
+      <c r="E49" s="100"/>
       <c r="F49" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G49" s="22"/>
-      <c r="H49" s="123"/>
-      <c r="I49" s="124"/>
+      <c r="H49" s="152"/>
+      <c r="I49" s="153"/>
     </row>
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3288,6 +3271,21 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated proposals, and destinations
</commit_message>
<xml_diff>
--- a/CS320-Spring2022Calendar-original(1-28-22).xlsx
+++ b/CS320-Spring2022Calendar-original(1-28-22).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523F1469-6458-472C-81EB-41692555CD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E3B8DC-71E4-41B5-A640-AD8B4B2D063F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9192" yWindow="324" windowWidth="13758" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1896" yWindow="456" windowWidth="19530" windowHeight="11754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp22" sheetId="1" r:id="rId1"/>
@@ -196,11 +196,6 @@
   </si>
   <si>
     <t>A01: Team Project Proposal due
-7:00 am
-(Google Doc)</t>
-  </si>
-  <si>
-    <t>A02: Individual Project Proposal due
 7:00 am
 (Google Doc)</t>
   </si>
@@ -566,8 +561,13 @@
     </r>
   </si>
   <si>
+    <t>A02: Individual Project Proposal due
+7:00 am
+(Marmoset)</t>
+  </si>
+  <si>
     <t>CS320: SW Engineering - Spring 2022 Schedule
-(as of 12-29-2021, subject to change)</t>
+(as of 1-23-2022, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1652,35 +1652,17 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1688,6 +1670,60 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1698,42 +1734,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2079,8 +2079,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2098,17 +2098,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="128"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
@@ -2138,10 +2138,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="132">
+      <c r="A3" s="138">
         <v>15</v>
       </c>
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="129" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="113">
@@ -2173,8 +2173,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="131"/>
-      <c r="B4" s="148"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="132"/>
       <c r="C4" s="115" t="s">
         <v>8</v>
       </c>
@@ -2200,12 +2200,12 @@
       <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="131">
+      <c r="A5" s="139">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="136" t="s">
-        <v>57</v>
+      <c r="B5" s="130" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="8">
         <f>I3 + 1</f>
@@ -2236,30 +2236,30 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="133"/>
-      <c r="B6" s="137"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="68"/>
       <c r="D6" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="86"/>
       <c r="F6" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="67" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="134">
+      <c r="A7" s="143">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="150" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="51">
@@ -2292,32 +2292,32 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="135"/>
-      <c r="B8" s="139"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="151"/>
       <c r="C8" s="40" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="67" t="s">
         <v>40</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="135">
+      <c r="A9" s="136">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="139"/>
+      <c r="B9" s="151"/>
       <c r="C9" s="15">
         <f>I7 + 1</f>
         <v>13</v>
@@ -2348,10 +2348,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="135"/>
-      <c r="B10" s="139"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="151"/>
       <c r="C10" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="48" t="s">
         <v>25</v>
@@ -2367,11 +2367,11 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="135">
+      <c r="A11" s="136">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="139"/>
+      <c r="B11" s="151"/>
       <c r="C11" s="18">
         <f>I9 + 1</f>
         <v>20</v>
@@ -2402,8 +2402,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="90.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="135"/>
-      <c r="B12" s="139"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="151"/>
       <c r="C12" s="38"/>
       <c r="D12" s="13" t="s">
         <v>34</v>
@@ -2413,18 +2413,18 @@
         <v>36</v>
       </c>
       <c r="G12" s="85"/>
-      <c r="H12" s="153" t="s">
+      <c r="H12" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="152"/>
+      <c r="I12" s="126"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="140">
+      <c r="A13" s="152">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="149" t="s">
-        <v>58</v>
+      <c r="B13" s="133" t="s">
+        <v>57</v>
       </c>
       <c r="C13" s="18">
         <f>I11 + 1</f>
@@ -2455,28 +2455,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="141"/>
-      <c r="B14" s="150"/>
+      <c r="A14" s="153"/>
+      <c r="B14" s="134"/>
       <c r="C14" s="38"/>
       <c r="D14" s="103" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="82"/>
       <c r="F14" s="64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" s="78"/>
       <c r="H14" s="49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="132">
+      <c r="A15" s="138">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="136" t="s">
+      <c r="B15" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="74">
@@ -2509,22 +2509,22 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="133"/>
-      <c r="B16" s="137"/>
+      <c r="A16" s="142"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="100" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="118" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="119" t="str">
         <f>G16</f>
@@ -2614,7 +2614,7 @@
       <c r="C23" s="41"/>
       <c r="D23" s="30"/>
       <c r="E23" s="99" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -2666,19 +2666,19 @@
       <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="126" t="str">
+      <c r="A28" s="145" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2022 Schedule
-(as of 12-29-2021, subject to change)</v>
-      </c>
-      <c r="B28" s="127"/>
-      <c r="C28" s="127"/>
-      <c r="D28" s="127"/>
-      <c r="E28" s="127"/>
-      <c r="F28" s="127"/>
-      <c r="G28" s="127"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="128"/>
+(as of 1-23-2022, subject to change)</v>
+      </c>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="146"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="146"/>
+      <c r="G28" s="146"/>
+      <c r="H28" s="146"/>
+      <c r="I28" s="147"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A29" s="1" t="str">
@@ -2716,11 +2716,11 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="129">
+      <c r="A30" s="148">
         <f>A15</f>
         <v>9</v>
       </c>
-      <c r="B30" s="147" t="s">
+      <c r="B30" s="129" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="87">
@@ -2753,8 +2753,8 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="130"/>
-      <c r="B31" s="136"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="87" t="str">
         <f>C16</f>
         <v xml:space="preserve"> </v>
@@ -2788,11 +2788,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="130">
+      <c r="A32" s="149">
         <f xml:space="preserve"> A30 - 1</f>
         <v>8</v>
       </c>
-      <c r="B32" s="136"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="112">
         <f>I15 + 1</f>
         <v>13</v>
@@ -2823,10 +2823,10 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="131"/>
-      <c r="B33" s="136"/>
+      <c r="A33" s="139"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>15</v>
@@ -2842,11 +2842,11 @@
       <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="131">
+      <c r="A34" s="139">
         <f>A32 - 1</f>
         <v>7</v>
       </c>
-      <c r="B34" s="136"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="21">
         <f>I32 + 1</f>
         <v>20</v>
@@ -2877,29 +2877,29 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="120.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A35" s="131"/>
-      <c r="B35" s="136"/>
+      <c r="A35" s="139"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="66"/>
       <c r="D35" s="33" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="80"/>
       <c r="F35" s="60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G35" s="66"/>
       <c r="H35" s="101" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I35" s="94"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="131">
+      <c r="A36" s="139">
         <f>A34 - 1</f>
         <v>6</v>
       </c>
-      <c r="B36" s="151" t="s">
-        <v>59</v>
+      <c r="B36" s="135" t="s">
+        <v>58</v>
       </c>
       <c r="C36" s="8">
         <f>I34 + 1</f>
@@ -2930,30 +2930,30 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="133"/>
-      <c r="B37" s="137"/>
+      <c r="A37" s="142"/>
+      <c r="B37" s="131"/>
       <c r="C37" s="93"/>
       <c r="D37" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E37" s="67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="94"/>
       <c r="H37" s="105" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="134">
+      <c r="A38" s="143">
         <f>A36 -1</f>
         <v>5</v>
       </c>
-      <c r="B38" s="146" t="s">
+      <c r="B38" s="128" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="91">
@@ -2986,30 +2986,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="135"/>
-      <c r="B39" s="146"/>
+      <c r="A39" s="136"/>
+      <c r="B39" s="128"/>
       <c r="C39" s="96"/>
       <c r="D39" s="33" t="s">
         <v>38</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G39" s="104"/>
       <c r="H39" s="102" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I39" s="37"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="145">
+      <c r="A40" s="144">
         <f>A38 -1</f>
         <v>4</v>
       </c>
-      <c r="B40" s="146"/>
+      <c r="B40" s="128"/>
       <c r="C40" s="95">
         <f>I38 + 1</f>
         <v>10</v>
@@ -3040,8 +3040,8 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="44.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="135"/>
-      <c r="B41" s="146"/>
+      <c r="A41" s="136"/>
+      <c r="B41" s="128"/>
       <c r="C41" s="38"/>
       <c r="D41" s="36" t="s">
         <v>7</v>
@@ -3059,11 +3059,11 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="135">
+      <c r="A42" s="136">
         <f>A40 -1</f>
         <v>3</v>
       </c>
-      <c r="B42" s="146"/>
+      <c r="B42" s="128"/>
       <c r="C42" s="110">
         <f>I40 + 1</f>
         <v>17</v>
@@ -3094,8 +3094,8 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="135"/>
-      <c r="B43" s="146"/>
+      <c r="A43" s="136"/>
+      <c r="B43" s="128"/>
       <c r="C43" s="115" t="s">
         <v>6</v>
       </c>
@@ -3113,11 +3113,11 @@
       <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="135">
+      <c r="A44" s="136">
         <f>A42 -1</f>
         <v>2</v>
       </c>
-      <c r="B44" s="146"/>
+      <c r="B44" s="128"/>
       <c r="C44" s="38">
         <f>I42 + 1</f>
         <v>24</v>
@@ -3148,8 +3148,8 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="142"/>
-      <c r="B45" s="146"/>
+      <c r="A45" s="137"/>
+      <c r="B45" s="128"/>
       <c r="C45" s="88"/>
       <c r="D45" s="57"/>
       <c r="E45" s="55"/>
@@ -3163,11 +3163,11 @@
       <c r="I45" s="54"/>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="132">
+      <c r="A46" s="138">
         <f>A44 -1</f>
         <v>1</v>
       </c>
-      <c r="B46" s="147" t="s">
+      <c r="B46" s="129" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="34">
@@ -3199,8 +3199,8 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="131"/>
-      <c r="B47" s="136"/>
+      <c r="A47" s="139"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="35"/>
       <c r="D47" s="7" t="s">
         <v>7</v>
@@ -3211,17 +3211,17 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="143" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="136"/>
+      <c r="A48" s="140" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="130"/>
       <c r="C48" s="21">
         <f>I46 + 1</f>
         <v>8</v>
@@ -3252,17 +3252,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A49" s="144"/>
-      <c r="B49" s="137"/>
+      <c r="A49" s="141"/>
+      <c r="B49" s="131"/>
       <c r="C49" s="97" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E49" s="98"/>
       <c r="F49" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="124"/>
@@ -3271,21 +3271,6 @@
     <row r="50" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B38:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -3299,6 +3284,21 @@
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B38:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="5" scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>